<commit_message>
somehow hit rate fixed
</commit_message>
<xml_diff>
--- a/Cache_Impliment/Cache/Cache/Trend_Dump.xlsx
+++ b/Cache_Impliment/Cache/Cache/Trend_Dump.xlsx
@@ -504,11 +504,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236530864"/>
-        <c:axId val="236531424"/>
+        <c:axId val="153882304"/>
+        <c:axId val="153882864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236530864"/>
+        <c:axId val="153882304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +551,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236531424"/>
+        <c:crossAx val="153882864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -559,7 +559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236531424"/>
+        <c:axId val="153882864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +610,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236530864"/>
+        <c:crossAx val="153882304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -892,11 +892,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236534784"/>
-        <c:axId val="236535344"/>
+        <c:axId val="156921600"/>
+        <c:axId val="156930000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236534784"/>
+        <c:axId val="156921600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,7 +939,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236535344"/>
+        <c:crossAx val="156930000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -947,7 +947,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236535344"/>
+        <c:axId val="156930000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,7 +998,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236534784"/>
+        <c:crossAx val="156921600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1275,11 +1275,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236933392"/>
-        <c:axId val="236933952"/>
+        <c:axId val="239033968"/>
+        <c:axId val="239034528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236933392"/>
+        <c:axId val="239033968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236933952"/>
+        <c:crossAx val="239034528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1330,7 +1330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236933952"/>
+        <c:axId val="239034528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1381,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236933392"/>
+        <c:crossAx val="239033968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1662,11 +1662,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236937312"/>
-        <c:axId val="236937872"/>
+        <c:axId val="239037888"/>
+        <c:axId val="239038448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236937312"/>
+        <c:axId val="239037888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236937872"/>
+        <c:crossAx val="239038448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1717,7 +1717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236937872"/>
+        <c:axId val="239038448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +1768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236937312"/>
+        <c:crossAx val="239037888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4485,7 +4485,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V42" sqref="V42"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4612,7 +4612,7 @@
         <v>100230049</v>
       </c>
       <c r="C4" s="1">
-        <v>100230049</v>
+        <v>95191124</v>
       </c>
       <c r="D4" s="1">
         <v>90.737899999999996</v>
@@ -4622,20 +4622,20 @@
         <v>433284589</v>
       </c>
       <c r="G4" s="1">
-        <v>100230049</v>
+        <v>648862226</v>
       </c>
       <c r="H4" s="1">
-        <v>100230049</v>
+        <v>648859317</v>
       </c>
       <c r="I4" s="1">
         <v>40.039400000000001</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
-        <v>100230049</v>
+        <v>11250430</v>
       </c>
       <c r="L4" s="12">
-        <v>100230049</v>
+        <v>5613899</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -4748,7 +4748,7 @@
         <v>27492371</v>
       </c>
       <c r="C8" s="2">
-        <v>27492371</v>
+        <v>26625618</v>
       </c>
       <c r="D8" s="2">
         <v>97.459500000000006</v>
@@ -4758,20 +4758,20 @@
         <v>530545180</v>
       </c>
       <c r="G8" s="2">
-        <v>27492371</v>
+        <v>551601635</v>
       </c>
       <c r="H8" s="2">
-        <v>27492371</v>
+        <v>551600791</v>
       </c>
       <c r="I8" s="2">
         <v>49.027099999999997</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2">
-        <v>27492371</v>
+        <v>11250430</v>
       </c>
       <c r="L8" s="14">
-        <v>27492371</v>
+        <v>5597781</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -4884,7 +4884,7 @@
         <v>1888678</v>
       </c>
       <c r="C12" s="3">
-        <v>1888678</v>
+        <v>271058</v>
       </c>
       <c r="D12" s="3">
         <v>99.825500000000005</v>
@@ -4894,20 +4894,20 @@
         <v>1079334144</v>
       </c>
       <c r="G12" s="3">
-        <v>1888678</v>
+        <v>2812671</v>
       </c>
       <c r="H12" s="3">
-        <v>1888678</v>
+        <v>2812578</v>
       </c>
       <c r="I12" s="3">
         <v>99.740099999999998</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3">
-        <v>1888678</v>
+        <v>11250430</v>
       </c>
       <c r="L12" s="16">
-        <v>1888678</v>
+        <v>395500</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>82610948</v>
       </c>
       <c r="C16" s="4">
-        <v>82610948</v>
+        <v>81495232</v>
       </c>
       <c r="D16" s="4">
         <v>92.366</v>
@@ -5030,20 +5030,20 @@
         <v>491206524</v>
       </c>
       <c r="G16" s="4">
-        <v>82610948</v>
+        <v>590940291</v>
       </c>
       <c r="H16" s="4">
-        <v>82610948</v>
+        <v>590934748</v>
       </c>
       <c r="I16" s="4">
         <v>45.3919</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4">
-        <v>82610948</v>
+        <v>11250430</v>
       </c>
       <c r="L16" s="18">
-        <v>82610948</v>
+        <v>5613744</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -5156,7 +5156,7 @@
         <v>24798457</v>
       </c>
       <c r="C20" s="5">
-        <v>24798457</v>
+        <v>24509011</v>
       </c>
       <c r="D20" s="5">
         <v>97.708399999999997</v>
@@ -5166,20 +5166,20 @@
         <v>819560390</v>
       </c>
       <c r="G20" s="5">
-        <v>24798457</v>
+        <v>262586425</v>
       </c>
       <c r="H20" s="5">
-        <v>24798457</v>
+        <v>262584698</v>
       </c>
       <c r="I20" s="5">
         <v>75.734700000000004</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5">
-        <v>24798457</v>
+        <v>11250430</v>
       </c>
       <c r="L20" s="20">
-        <v>24798457</v>
+        <v>5597453</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -5292,7 +5292,7 @@
         <v>472248</v>
       </c>
       <c r="C24" s="7">
-        <v>472248</v>
+        <v>251135</v>
       </c>
       <c r="D24" s="7">
         <v>99.956400000000002</v>
@@ -5302,20 +5302,20 @@
         <v>1081443520</v>
       </c>
       <c r="G24" s="7">
-        <v>472248</v>
+        <v>703295</v>
       </c>
       <c r="H24" s="7">
-        <v>472248</v>
+        <v>703263</v>
       </c>
       <c r="I24" s="7">
         <v>99.935000000000002</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7">
-        <v>472248</v>
+        <v>11250430</v>
       </c>
       <c r="L24" s="24">
-        <v>472248</v>
+        <v>392073</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -5432,7 +5432,7 @@
         <v>60261595</v>
       </c>
       <c r="C28" s="1">
-        <v>60261595</v>
+        <v>57195124</v>
       </c>
       <c r="D28" s="1">
         <v>94.431299999999993</v>
@@ -5445,10 +5445,10 @@
         <v>457671604</v>
       </c>
       <c r="G28" s="1">
-        <v>60261595</v>
+        <v>624475211</v>
       </c>
       <c r="H28" s="1">
-        <v>60261595</v>
+        <v>624473369</v>
       </c>
       <c r="I28" s="1">
         <v>42.292900000000003</v>
@@ -5458,10 +5458,10 @@
         <v>1.0562820621687639</v>
       </c>
       <c r="K28" s="1">
-        <v>60261595</v>
+        <v>11250430</v>
       </c>
       <c r="L28" s="12">
-        <v>60261595</v>
+        <v>5584490</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -5578,7 +5578,7 @@
         <v>15907892</v>
       </c>
       <c r="C32" s="2">
-        <v>15907892</v>
+        <v>15395621</v>
       </c>
       <c r="D32" s="2">
         <v>98.53</v>
@@ -5591,10 +5591,10 @@
         <v>540257104</v>
       </c>
       <c r="G32" s="2">
-        <v>15907892</v>
+        <v>541889711</v>
       </c>
       <c r="H32" s="2">
-        <v>15907892</v>
+        <v>541889183</v>
       </c>
       <c r="I32" s="2">
         <v>49.924599999999998</v>
@@ -5604,10 +5604,10 @@
         <v>1.0183062020800742</v>
       </c>
       <c r="K32" s="2">
-        <v>15907892</v>
+        <v>11250430</v>
       </c>
       <c r="L32" s="14">
-        <v>15907892</v>
+        <v>5331209</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -5724,7 +5724,7 @@
         <v>2028307</v>
       </c>
       <c r="C36" s="3">
-        <v>2028307</v>
+        <v>415054</v>
       </c>
       <c r="D36" s="3">
         <v>99.812600000000003</v>
@@ -5737,10 +5737,10 @@
         <v>1078377120</v>
       </c>
       <c r="G36" s="3">
-        <v>2028307</v>
+        <v>3769695</v>
       </c>
       <c r="H36" s="3">
-        <v>2028307</v>
+        <v>3769601</v>
       </c>
       <c r="I36" s="3">
         <v>99.651600000000002</v>
@@ -5750,10 +5750,10 @@
         <v>0.99911269389142388</v>
       </c>
       <c r="K36" s="3">
-        <v>2028307</v>
+        <v>11250430</v>
       </c>
       <c r="L36" s="16">
-        <v>2028307</v>
+        <v>833168</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -5870,7 +5870,7 @@
         <v>43389861</v>
       </c>
       <c r="C40" s="4">
-        <v>43389861</v>
+        <v>43061838</v>
       </c>
       <c r="D40" s="4">
         <v>95.990399999999994</v>
@@ -5883,10 +5883,10 @@
         <v>646950326</v>
       </c>
       <c r="G40" s="4">
-        <v>43389861</v>
+        <v>435196489</v>
       </c>
       <c r="H40" s="4">
-        <v>43389861</v>
+        <v>435193716</v>
       </c>
       <c r="I40" s="4">
         <v>59.783999999999999</v>
@@ -5896,10 +5896,10 @@
         <v>1.3170631764698106</v>
       </c>
       <c r="K40" s="4">
-        <v>43389861</v>
+        <v>11250430</v>
       </c>
       <c r="L40" s="18">
-        <v>43389861</v>
+        <v>5496181</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -6016,7 +6016,7 @@
         <v>5462221</v>
       </c>
       <c r="C44" s="5">
-        <v>5462221</v>
+        <v>5414183</v>
       </c>
       <c r="D44" s="5">
         <v>99.495199999999997</v>
@@ -6029,10 +6029,10 @@
         <v>887660245</v>
       </c>
       <c r="G44" s="5">
-        <v>5462221</v>
+        <v>194486570</v>
       </c>
       <c r="H44" s="5">
-        <v>5462221</v>
+        <v>194485958</v>
       </c>
       <c r="I44" s="5">
         <v>82.027699999999996</v>
@@ -6042,10 +6042,10 @@
         <v>1.0830926906688743</v>
       </c>
       <c r="K44" s="5">
-        <v>5462221</v>
+        <v>11250430</v>
       </c>
       <c r="L44" s="20">
-        <v>5462221</v>
+        <v>4627080</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -6162,7 +6162,7 @@
         <v>502611</v>
       </c>
       <c r="C48" s="7">
-        <v>502611</v>
+        <v>283048</v>
       </c>
       <c r="D48" s="7">
         <v>99.953599999999994</v>
@@ -6175,10 +6175,10 @@
         <v>1081220249</v>
       </c>
       <c r="G48" s="7">
-        <v>502611</v>
+        <v>926566</v>
       </c>
       <c r="H48" s="7">
-        <v>502611</v>
+        <v>926534</v>
       </c>
       <c r="I48" s="7">
         <v>99.914400000000001</v>
@@ -6188,16 +6188,15 @@
         <v>0.99979386601290843</v>
       </c>
       <c r="K48" s="7">
-        <v>502611</v>
+        <v>11250430</v>
       </c>
       <c r="L48" s="24">
-        <v>502611</v>
+        <v>513581</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6366,7 +6365,7 @@
       </c>
       <c r="C4" s="1">
         <f>Ways!C4</f>
-        <v>100230049</v>
+        <v>95191124</v>
       </c>
       <c r="D4" s="1">
         <f>Ways!D4</f>
@@ -6379,11 +6378,11 @@
       </c>
       <c r="G4" s="1">
         <f>Ways!G4</f>
-        <v>100230049</v>
+        <v>648862226</v>
       </c>
       <c r="H4" s="1">
         <f>Ways!H4</f>
-        <v>100230049</v>
+        <v>648859317</v>
       </c>
       <c r="I4" s="1">
         <f>Ways!I4</f>
@@ -6392,11 +6391,11 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1">
         <f>Ways!K4</f>
-        <v>100230049</v>
+        <v>11250430</v>
       </c>
       <c r="L4" s="12">
         <f>Ways!L4</f>
-        <v>100230049</v>
+        <v>5613899</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6542,7 +6541,7 @@
       </c>
       <c r="C8" s="2">
         <f>Ways!C8</f>
-        <v>27492371</v>
+        <v>26625618</v>
       </c>
       <c r="D8" s="2">
         <f>Ways!D8</f>
@@ -6555,11 +6554,11 @@
       </c>
       <c r="G8" s="2">
         <f>Ways!G8</f>
-        <v>27492371</v>
+        <v>551601635</v>
       </c>
       <c r="H8" s="2">
         <f>Ways!H8</f>
-        <v>27492371</v>
+        <v>551600791</v>
       </c>
       <c r="I8" s="2">
         <f>Ways!I8</f>
@@ -6568,11 +6567,11 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2">
         <f>Ways!K8</f>
-        <v>27492371</v>
+        <v>11250430</v>
       </c>
       <c r="L8" s="14">
         <f>Ways!L8</f>
-        <v>27492371</v>
+        <v>5597781</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6718,7 +6717,7 @@
       </c>
       <c r="C12" s="3">
         <f>Ways!C12</f>
-        <v>1888678</v>
+        <v>271058</v>
       </c>
       <c r="D12" s="3">
         <f>Ways!D12</f>
@@ -6731,11 +6730,11 @@
       </c>
       <c r="G12" s="3">
         <f>Ways!G12</f>
-        <v>1888678</v>
+        <v>2812671</v>
       </c>
       <c r="H12" s="3">
         <f>Ways!H12</f>
-        <v>1888678</v>
+        <v>2812578</v>
       </c>
       <c r="I12" s="3">
         <f>Ways!I12</f>
@@ -6744,11 +6743,11 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3">
         <f>Ways!K12</f>
-        <v>1888678</v>
+        <v>11250430</v>
       </c>
       <c r="L12" s="16">
         <f>Ways!L12</f>
-        <v>1888678</v>
+        <v>395500</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6894,7 +6893,7 @@
       </c>
       <c r="C16" s="4">
         <f>Ways!C16</f>
-        <v>82610948</v>
+        <v>81495232</v>
       </c>
       <c r="D16" s="4">
         <f>Ways!D16</f>
@@ -6910,11 +6909,11 @@
       </c>
       <c r="G16" s="4">
         <f>Ways!G16</f>
-        <v>82610948</v>
+        <v>590940291</v>
       </c>
       <c r="H16" s="4">
         <f>Ways!H16</f>
-        <v>82610948</v>
+        <v>590934748</v>
       </c>
       <c r="I16" s="4">
         <f>Ways!I16</f>
@@ -6926,11 +6925,11 @@
       </c>
       <c r="K16" s="4">
         <f>Ways!K16</f>
-        <v>82610948</v>
+        <v>11250430</v>
       </c>
       <c r="L16" s="18">
         <f>Ways!L16</f>
-        <v>82610948</v>
+        <v>5613744</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -7076,7 +7075,7 @@
       </c>
       <c r="C20" s="5">
         <f>Ways!C20</f>
-        <v>24798457</v>
+        <v>24509011</v>
       </c>
       <c r="D20" s="5">
         <f>Ways!D20</f>
@@ -7092,11 +7091,11 @@
       </c>
       <c r="G20" s="5">
         <f>Ways!G20</f>
-        <v>24798457</v>
+        <v>262586425</v>
       </c>
       <c r="H20" s="5">
         <f>Ways!H20</f>
-        <v>24798457</v>
+        <v>262584698</v>
       </c>
       <c r="I20" s="5">
         <f>Ways!I20</f>
@@ -7108,11 +7107,11 @@
       </c>
       <c r="K20" s="5">
         <f>Ways!K20</f>
-        <v>24798457</v>
+        <v>11250430</v>
       </c>
       <c r="L20" s="20">
         <f>Ways!L20</f>
-        <v>24798457</v>
+        <v>5597453</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -7258,7 +7257,7 @@
       </c>
       <c r="C24" s="7">
         <f>Ways!C24</f>
-        <v>472248</v>
+        <v>251135</v>
       </c>
       <c r="D24" s="7">
         <f>Ways!D24</f>
@@ -7274,11 +7273,11 @@
       </c>
       <c r="G24" s="7">
         <f>Ways!G24</f>
-        <v>472248</v>
+        <v>703295</v>
       </c>
       <c r="H24" s="7">
         <f>Ways!H24</f>
-        <v>472248</v>
+        <v>703263</v>
       </c>
       <c r="I24" s="7">
         <f>Ways!I24</f>
@@ -7290,11 +7289,11 @@
       </c>
       <c r="K24" s="7">
         <f>Ways!K24</f>
-        <v>472248</v>
+        <v>11250430</v>
       </c>
       <c r="L24" s="24">
         <f>Ways!L24</f>
-        <v>472248</v>
+        <v>392073</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -7440,7 +7439,7 @@
       </c>
       <c r="C28" s="1">
         <f>Ways!C28</f>
-        <v>60261595</v>
+        <v>57195124</v>
       </c>
       <c r="D28" s="1">
         <f>Ways!D28</f>
@@ -7453,11 +7452,11 @@
       </c>
       <c r="G28" s="1">
         <f>Ways!G28</f>
-        <v>60261595</v>
+        <v>624475211</v>
       </c>
       <c r="H28" s="1">
         <f>Ways!H28</f>
-        <v>60261595</v>
+        <v>624473369</v>
       </c>
       <c r="I28" s="1">
         <f>Ways!I28</f>
@@ -7466,11 +7465,11 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1">
         <f>Ways!K28</f>
-        <v>60261595</v>
+        <v>11250430</v>
       </c>
       <c r="L28" s="12">
         <f>Ways!L28</f>
-        <v>60261595</v>
+        <v>5584490</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -7616,7 +7615,7 @@
       </c>
       <c r="C32" s="2">
         <f>Ways!C32</f>
-        <v>15907892</v>
+        <v>15395621</v>
       </c>
       <c r="D32" s="2">
         <f>Ways!D32</f>
@@ -7629,11 +7628,11 @@
       </c>
       <c r="G32" s="2">
         <f>Ways!G32</f>
-        <v>15907892</v>
+        <v>541889711</v>
       </c>
       <c r="H32" s="2">
         <f>Ways!H32</f>
-        <v>15907892</v>
+        <v>541889183</v>
       </c>
       <c r="I32" s="2">
         <f>Ways!I32</f>
@@ -7642,11 +7641,11 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2">
         <f>Ways!K32</f>
-        <v>15907892</v>
+        <v>11250430</v>
       </c>
       <c r="L32" s="14">
         <f>Ways!L32</f>
-        <v>15907892</v>
+        <v>5331209</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -7792,7 +7791,7 @@
       </c>
       <c r="C36" s="3">
         <f>Ways!C36</f>
-        <v>2028307</v>
+        <v>415054</v>
       </c>
       <c r="D36" s="3">
         <f>Ways!D36</f>
@@ -7805,11 +7804,11 @@
       </c>
       <c r="G36" s="3">
         <f>Ways!G36</f>
-        <v>2028307</v>
+        <v>3769695</v>
       </c>
       <c r="H36" s="3">
         <f>Ways!H36</f>
-        <v>2028307</v>
+        <v>3769601</v>
       </c>
       <c r="I36" s="3">
         <f>Ways!I36</f>
@@ -7818,11 +7817,11 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3">
         <f>Ways!K36</f>
-        <v>2028307</v>
+        <v>11250430</v>
       </c>
       <c r="L36" s="16">
         <f>Ways!L36</f>
-        <v>2028307</v>
+        <v>833168</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -7968,7 +7967,7 @@
       </c>
       <c r="C40" s="4">
         <f>Ways!C40</f>
-        <v>43389861</v>
+        <v>43061838</v>
       </c>
       <c r="D40" s="4">
         <f>Ways!D40</f>
@@ -7984,11 +7983,11 @@
       </c>
       <c r="G40" s="4">
         <f>Ways!G40</f>
-        <v>43389861</v>
+        <v>435196489</v>
       </c>
       <c r="H40" s="4">
         <f>Ways!H40</f>
-        <v>43389861</v>
+        <v>435193716</v>
       </c>
       <c r="I40" s="4">
         <f>Ways!I40</f>
@@ -8000,11 +7999,11 @@
       </c>
       <c r="K40" s="4">
         <f>Ways!K40</f>
-        <v>43389861</v>
+        <v>11250430</v>
       </c>
       <c r="L40" s="18">
         <f>Ways!L40</f>
-        <v>43389861</v>
+        <v>5496181</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -8150,7 +8149,7 @@
       </c>
       <c r="C44" s="5">
         <f>Ways!C44</f>
-        <v>5462221</v>
+        <v>5414183</v>
       </c>
       <c r="D44" s="5">
         <f>Ways!D44</f>
@@ -8166,11 +8165,11 @@
       </c>
       <c r="G44" s="5">
         <f>Ways!G44</f>
-        <v>5462221</v>
+        <v>194486570</v>
       </c>
       <c r="H44" s="5">
         <f>Ways!H44</f>
-        <v>5462221</v>
+        <v>194485958</v>
       </c>
       <c r="I44" s="5">
         <f>Ways!I44</f>
@@ -8182,11 +8181,11 @@
       </c>
       <c r="K44" s="5">
         <f>Ways!K44</f>
-        <v>5462221</v>
+        <v>11250430</v>
       </c>
       <c r="L44" s="20">
         <f>Ways!L44</f>
-        <v>5462221</v>
+        <v>4627080</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -8332,7 +8331,7 @@
       </c>
       <c r="C48" s="7">
         <f>Ways!C48</f>
-        <v>502611</v>
+        <v>283048</v>
       </c>
       <c r="D48" s="7">
         <f>Ways!D48</f>
@@ -8348,11 +8347,11 @@
       </c>
       <c r="G48" s="7">
         <f>Ways!G48</f>
-        <v>502611</v>
+        <v>926566</v>
       </c>
       <c r="H48" s="7">
         <f>Ways!H48</f>
-        <v>502611</v>
+        <v>926534</v>
       </c>
       <c r="I48" s="7">
         <f>Ways!I48</f>
@@ -8364,11 +8363,11 @@
       </c>
       <c r="K48" s="7">
         <f>Ways!K48</f>
-        <v>502611</v>
+        <v>11250430</v>
       </c>
       <c r="L48" s="24">
         <f>Ways!L48</f>
-        <v>502611</v>
+        <v>513581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>